<commit_message>
added my project tracker
</commit_message>
<xml_diff>
--- a/Docs/Reports/Christopher_tracker.xlsx
+++ b/Docs/Reports/Christopher_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b18f37f46ca55066/Desktop/ISU/Fall 2025/RCET 3375/5th Final Project/Farm-Bureau-Project/Docs/Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="390" documentId="11_F25DC773A252ABDACC10485029DF4BCC5BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1723502-A744-4BDB-97D2-8ADA5A2E250E}"/>
+  <xr:revisionPtr revIDLastSave="403" documentId="11_F25DC773A252ABDACC10485029DF4BCC5BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0B9DAF1-1DBB-49A0-895A-511A3461DA29}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
   <si>
     <t>Day</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Whiteboard/brainstorm a process life cycle diagram.</t>
   </si>
   <si>
-    <t>Whiteboard/brainstorm serial comms and memory management scheme.</t>
-  </si>
-  <si>
     <t>n/a</t>
   </si>
   <si>
@@ -156,7 +153,25 @@
     <t>All goals were accomplished. I got the team together to map out I/O and to make selection of compenents we want to use. The parts were orderedby Shane and should be here after the Thanksgiving week.</t>
   </si>
   <si>
-    <t>All goals except PID code were completed. Noah and I were still finishing the I2C lab so most of the PIC coding was done by Jacob. I led a coule of brainstorming sessions to ensure that the team is aligned on how our firmware will control the hardware of the system. The team is still learning how to use the Github repo.</t>
+    <t>https://github.com/Christopher-isu/Farm-Bureau-Project/blob/main/IO_Block_diagram_v1.svg</t>
+  </si>
+  <si>
+    <t>https://github.com/Christopher-isu/Farm-Bureau-Project/blob/main/Docs/Whiteboard%20Sessions/IOscheme.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/Christopher-isu/Farm-Bureau-Project/blob/main/Docs/Whiteboard%20Sessions/MCU-UI-commStructure.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/Christopher-isu/Farm-Bureau-Project/blob/main/Docs/Whiteboard%20Sessions/process_cycle.jpg</t>
+  </si>
+  <si>
+    <t>Whiteboard/brainstorm serial comms implementation.</t>
+  </si>
+  <si>
+    <t>Whiteboard/brainstorm  memory management scheme.</t>
+  </si>
+  <si>
+    <t>All goals except PID code were completed. Noah and I were still finishing the I2C lab so most of the PIC coding was done by Jacob. I led a coule of brainstorming sessions to ensure that the team is aligned on how our firmware will control the hardware of the system. For PID control I got C code for PID math and now I need to implement it in PIC16F1788.</t>
   </si>
 </sst>
 </file>
@@ -166,7 +181,7 @@
   <numFmts count="1">
     <numFmt numFmtId="168" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +199,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -409,10 +432,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -500,8 +524,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -780,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.5546875" defaultRowHeight="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -812,7 +840,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="32" t="s">
         <v>26</v>
@@ -851,7 +879,7 @@
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="33" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D5" s="35" t="s">
         <v>25</v>
@@ -859,10 +887,12 @@
     </row>
     <row r="6" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
+      <c r="C6" s="33" t="s">
+        <v>43</v>
+      </c>
       <c r="D6" s="34"/>
     </row>
     <row r="7" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -885,30 +915,30 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="39" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D9" s="40"/>
     </row>
     <row r="10" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -924,19 +954,46 @@
     </row>
     <row r="12" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>35</v>
-      </c>
-    </row>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C14" s="31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C15" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="14.4" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A13" r:id="rId1" xr:uid="{79D3D91F-52CA-4902-BFB2-6734045D63B0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updated the tracker for week 5
</commit_message>
<xml_diff>
--- a/Docs/Reports/Christopher_tracker.xlsx
+++ b/Docs/Reports/Christopher_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b18f37f46ca55066/Desktop/ISU/Fall 2025/RCET 3375/5th Final Project/Farm-Bureau-Project/Docs/Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="403" documentId="11_F25DC773A252ABDACC10485029DF4BCC5BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0B9DAF1-1DBB-49A0-895A-511A3461DA29}"/>
+  <xr:revisionPtr revIDLastSave="418" documentId="11_F25DC773A252ABDACC10485029DF4BCC5BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2184AF2E-F1F9-4277-A38D-38CBF879B2CA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
   <si>
     <t>Day</t>
   </si>
@@ -99,12 +99,6 @@
     <t>Goals for the week two (Nov 24)</t>
   </si>
   <si>
-    <t>Goals for the week two (Dec 1)</t>
-  </si>
-  <si>
-    <t>Goals for the week two (Dec 8)</t>
-  </si>
-  <si>
     <t>Test PID code with heating element</t>
   </si>
   <si>
@@ -172,6 +166,24 @@
   </si>
   <si>
     <t>All goals except PID code were completed. Noah and I were still finishing the I2C lab so most of the PIC coding was done by Jacob. I led a coule of brainstorming sessions to ensure that the team is aligned on how our firmware will control the hardware of the system. For PID control I got C code for PID math and now I need to implement it in PIC16F1788.</t>
+  </si>
+  <si>
+    <t>Goals for the week three (Dec 1)</t>
+  </si>
+  <si>
+    <t>Goals for the week four (Dec 8)</t>
+  </si>
+  <si>
+    <t>Assemble the stand for the model.</t>
+  </si>
+  <si>
+    <t>Cut styrofoam for the landscape outline.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PID was put on hold due to complexiton of implementation on PIC16F1788 (considering all other processes already running on it).  We built the frame using rack shelving.  We assembled electronics test rig and verified operation by actuating each of the components. </t>
+  </si>
+  <si>
+    <t>Goals for the week five (Dec 15)</t>
   </si>
 </sst>
 </file>
@@ -179,7 +191,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -436,96 +448,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -543,6 +551,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -808,183 +820,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.5546875" defaultRowHeight="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.5546875" style="21"/>
-    <col min="2" max="4" width="42.5546875" style="31"/>
-    <col min="5" max="16384" width="42.5546875" style="20"/>
+    <col min="1" max="1" width="42.5546875" style="15"/>
+    <col min="2" max="5" width="42.5546875" style="25"/>
+    <col min="6" max="16384" width="42.5546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:5" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="E3" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="D4" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="B6" s="23"/>
+      <c r="C6" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="19"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="8" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="32" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="35" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="33" t="s">
+      <c r="C9" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="33"/>
+    </row>
+    <row r="10" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="29">
+        <v>9</v>
+      </c>
+      <c r="B11" s="30">
+        <v>0</v>
+      </c>
+      <c r="C11" s="30">
+        <v>11.5</v>
+      </c>
+      <c r="D11" s="37">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="35" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="34"/>
-    </row>
-    <row r="7" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="29"/>
-    </row>
-    <row r="8" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="38" t="s">
+      <c r="B12" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="40"/>
-    </row>
-    <row r="10" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="36">
-        <v>9</v>
-      </c>
-      <c r="B11" s="37">
-        <v>0</v>
-      </c>
-      <c r="C11" s="37">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="41" t="s">
+    </row>
+    <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C14" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="31" t="s">
+    </row>
+    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C15" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C14" s="31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C15" s="31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:5" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="17" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="18" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="19" ht="14.4" x14ac:dyDescent="0.3"/>
@@ -1031,450 +1075,437 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="1">
         <v>45978</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" s="10"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="35"/>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="1">
         <v>45979</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3">
         <v>1.5</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="35"/>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="1">
         <v>45980</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="35"/>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="1">
         <v>45981</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5">
         <v>2</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="35"/>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="1">
         <v>45982</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6">
         <v>2.5</v>
       </c>
-      <c r="E6" s="10"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="35"/>
+      <c r="B7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="11">
         <v>45983</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="16" t="s">
+      <c r="A8" s="35"/>
+      <c r="B8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="13">
         <v>45984</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="8">
         <v>0</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="9">
         <f>SUM(D2:D8)</f>
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="1">
         <v>45985</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9" s="10"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="35"/>
+      <c r="B10" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="1">
         <v>45986</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="35"/>
+      <c r="B11" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="1">
         <v>45987</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11">
         <v>0</v>
       </c>
-      <c r="E11" s="10"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8" t="s">
+      <c r="A12" s="35"/>
+      <c r="B12" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="1">
         <v>45988</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12">
         <v>0</v>
       </c>
-      <c r="E12" s="10"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="35"/>
+      <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="1">
         <v>45989</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13" s="10"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="14" t="s">
+      <c r="A14" s="35"/>
+      <c r="B14" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="11">
         <v>45990</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="16" t="s">
+      <c r="A15" s="35"/>
+      <c r="B15" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="13">
         <v>45991</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="8">
         <v>0</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="9">
         <f>SUM(D9:D15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="1">
         <v>45992</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16">
         <v>2.5</v>
       </c>
-      <c r="E16" s="10"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8" t="s">
+      <c r="A17" s="35"/>
+      <c r="B17" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="1">
         <v>45993</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17" s="10"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8" t="s">
+      <c r="A18" s="35"/>
+      <c r="B18" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="1">
         <v>45994</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18">
         <v>3</v>
       </c>
-      <c r="E18" s="10"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8" t="s">
+      <c r="A19" s="35"/>
+      <c r="B19" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="1">
         <v>45995</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19">
         <v>1</v>
       </c>
-      <c r="E19" s="10"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8" t="s">
+      <c r="A20" s="35"/>
+      <c r="B20" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="1">
         <v>45996</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20">
         <v>2</v>
       </c>
-      <c r="E20" s="10"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="14" t="s">
+      <c r="A21" s="35"/>
+      <c r="B21" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="11">
         <v>45997</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21">
         <v>0</v>
       </c>
-      <c r="E21" s="10"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="16" t="s">
+      <c r="A22" s="35"/>
+      <c r="B22" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="13">
         <v>45998</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="8">
         <v>2</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="9">
         <f>SUM(D16:D22)</f>
         <v>11.5</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="1">
         <v>45999</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="10"/>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8" t="s">
+      <c r="A24" s="35"/>
+      <c r="B24" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="1">
         <v>46000</v>
       </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="10"/>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8" t="s">
+      <c r="A25" s="35"/>
+      <c r="B25" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="1">
         <v>46001</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="10"/>
+      <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8" t="s">
+      <c r="A26" s="35"/>
+      <c r="B26" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="1">
         <v>46002</v>
       </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="10"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8" t="s">
+      <c r="A27" s="35"/>
+      <c r="B27" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="1">
         <v>46003</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="10"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
-      <c r="B28" s="14" t="s">
+      <c r="A28" s="35"/>
+      <c r="B28" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="11">
         <v>46004</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="10"/>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
-      <c r="B29" s="14" t="s">
+      <c r="A29" s="35"/>
+      <c r="B29" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="11">
         <v>46005</v>
       </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="10"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="1">
         <v>46006</v>
       </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="10"/>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
-      <c r="B31" s="8" t="s">
+      <c r="A31" s="35"/>
+      <c r="B31" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="1">
         <v>46007</v>
       </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="10"/>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
-      <c r="B32" s="8" t="s">
+      <c r="A32" s="35"/>
+      <c r="B32" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="1">
         <v>46008</v>
       </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="10"/>
+      <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8" t="s">
+      <c r="A33" s="35"/>
+      <c r="B33" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="1">
         <v>46009</v>
       </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
-      <c r="B34" s="8" t="s">
+      <c r="A34" s="35"/>
+      <c r="B34" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34" s="1">
         <v>46010</v>
       </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="10"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
-      <c r="B35" s="14" t="s">
+      <c r="A35" s="35"/>
+      <c r="B35" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="15">
+      <c r="C35" s="11">
         <v>46011</v>
       </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="10"/>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="11"/>
-      <c r="B36" s="16" t="s">
+      <c r="A36" s="36"/>
+      <c r="B36" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="17">
+      <c r="C36" s="13">
         <v>46012</v>
       </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="13"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
final update for this semester
</commit_message>
<xml_diff>
--- a/Docs/Reports/Christopher_tracker.xlsx
+++ b/Docs/Reports/Christopher_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b18f37f46ca55066/Desktop/ISU/Fall 2025/RCET 3375/5th Final Project/Farm-Bureau-Project/Docs/Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="540" documentId="11_F25DC773A252ABDACC10485029DF4BCC5BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{895A8278-247C-4F9D-BC07-7F43E81D893B}"/>
+  <xr:revisionPtr revIDLastSave="550" documentId="11_F25DC773A252ABDACC10485029DF4BCC5BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4BE1F6B-F082-4F4E-BFAD-DC6C154BD74A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
   <si>
     <t>Day</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>Second (holiday)</t>
+  </si>
+  <si>
+    <t>The structure was assembled as planned and was ready on time for the presentation. The landscape was minimalist with styrofoam outline but was sufficient to demonstrate the principle of operation. During tests and the presentation we have successfully cycled over all the process steps. PID was not included due to no sufficient time to finish implementation.</t>
+  </si>
+  <si>
+    <t>https://github.com/Christopher-isu/Farm-Bureau-Project.git</t>
   </si>
 </sst>
 </file>
@@ -507,7 +513,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -585,24 +591,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -612,6 +605,18 @@
     <xf numFmtId="164" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -899,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.5546875" defaultRowHeight="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1037,7 +1042,9 @@
       <c r="D9" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="33"/>
+      <c r="E9" s="33" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
@@ -1066,11 +1073,11 @@
       <c r="C11" s="30">
         <v>13.5</v>
       </c>
-      <c r="D11" s="35">
+      <c r="D11" s="30">
         <v>34</v>
       </c>
-      <c r="E11" s="25">
-        <v>20</v>
+      <c r="E11" s="30">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1096,6 +1103,9 @@
       </c>
       <c r="C13" s="25" t="s">
         <v>36</v>
+      </c>
+      <c r="E13" s="52" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1117,6 +1127,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A13" r:id="rId1" xr:uid="{79D3D91F-52CA-4902-BFB2-6734045D63B0}"/>
+    <hyperlink ref="E13" r:id="rId2" xr:uid="{3B2E8D39-9747-466E-BA66-5C9BE963B667}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1126,7 +1137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B6DEDB-7F77-4473-9875-A29B98AAB9EA}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A17" sqref="A17:A23"/>
     </sheetView>
   </sheetViews>
@@ -1138,21 +1149,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="39"/>
-      <c r="B1" s="40"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="40" t="s">
+      <c r="A1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="43" t="s">
+      <c r="E1" s="36"/>
+      <c r="F1" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="43" t="s">
+      <c r="G1" s="36"/>
+      <c r="H1" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="42"/>
+      <c r="I1" s="38"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -1184,7 +1195,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="49" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
@@ -1204,7 +1215,7 @@
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="36"/>
+      <c r="A4" s="49"/>
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -1219,13 +1230,13 @@
         <v>5</v>
       </c>
       <c r="G4" s="7"/>
-      <c r="H4" s="38">
+      <c r="H4">
         <v>2</v>
       </c>
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
+      <c r="A5" s="49"/>
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -1240,13 +1251,13 @@
         <v>6.5</v>
       </c>
       <c r="G5" s="7"/>
-      <c r="H5" s="38">
+      <c r="H5">
         <v>3</v>
       </c>
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
+      <c r="A6" s="49"/>
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -1261,13 +1272,13 @@
         <v>5</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="H6" s="38">
+      <c r="H6">
         <v>2</v>
       </c>
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="36"/>
+      <c r="A7" s="49"/>
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -1282,13 +1293,13 @@
         <v>6.5</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="H7" s="38">
+      <c r="H7">
         <v>2</v>
       </c>
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
+      <c r="A8" s="49"/>
       <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
@@ -1306,7 +1317,7 @@
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="36"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="12" t="s">
         <v>7</v>
       </c>
@@ -1334,151 +1345,151 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="41">
         <v>45985</v>
       </c>
-      <c r="D10" s="45">
-        <v>0</v>
-      </c>
-      <c r="E10" s="47"/>
-      <c r="F10" s="45">
-        <v>0</v>
-      </c>
-      <c r="G10" s="47"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="47"/>
+      <c r="D10" s="40">
+        <v>0</v>
+      </c>
+      <c r="E10" s="42"/>
+      <c r="F10" s="40">
+        <v>0</v>
+      </c>
+      <c r="G10" s="42"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="42"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="44"/>
-      <c r="B11" s="45" t="s">
+      <c r="A11" s="50"/>
+      <c r="B11" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11" s="41">
         <v>45986</v>
       </c>
-      <c r="D11" s="45">
-        <v>0</v>
-      </c>
-      <c r="E11" s="47"/>
-      <c r="F11" s="45">
-        <v>0</v>
-      </c>
-      <c r="G11" s="47"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="47"/>
+      <c r="D11" s="40">
+        <v>0</v>
+      </c>
+      <c r="E11" s="42"/>
+      <c r="F11" s="40">
+        <v>0</v>
+      </c>
+      <c r="G11" s="42"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="42"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="44"/>
-      <c r="B12" s="45" t="s">
+      <c r="A12" s="50"/>
+      <c r="B12" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="46">
+      <c r="C12" s="41">
         <v>45987</v>
       </c>
-      <c r="D12" s="45">
-        <v>0</v>
-      </c>
-      <c r="E12" s="47"/>
-      <c r="F12" s="45">
-        <v>0</v>
-      </c>
-      <c r="G12" s="47"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="47"/>
+      <c r="D12" s="40">
+        <v>0</v>
+      </c>
+      <c r="E12" s="42"/>
+      <c r="F12" s="40">
+        <v>0</v>
+      </c>
+      <c r="G12" s="42"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="42"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="44"/>
-      <c r="B13" s="45" t="s">
+      <c r="A13" s="50"/>
+      <c r="B13" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="41">
         <v>45988</v>
       </c>
-      <c r="D13" s="45">
-        <v>0</v>
-      </c>
-      <c r="E13" s="47"/>
-      <c r="F13" s="45">
-        <v>0</v>
-      </c>
-      <c r="G13" s="47"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="47"/>
+      <c r="D13" s="40">
+        <v>0</v>
+      </c>
+      <c r="E13" s="42"/>
+      <c r="F13" s="40">
+        <v>0</v>
+      </c>
+      <c r="G13" s="42"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="42"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="44"/>
-      <c r="B14" s="45" t="s">
+      <c r="A14" s="50"/>
+      <c r="B14" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="41">
         <v>45989</v>
       </c>
-      <c r="D14" s="45">
-        <v>0</v>
-      </c>
-      <c r="E14" s="47"/>
-      <c r="F14" s="45">
-        <v>0</v>
-      </c>
-      <c r="G14" s="47"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="47"/>
+      <c r="D14" s="40">
+        <v>0</v>
+      </c>
+      <c r="E14" s="42"/>
+      <c r="F14" s="40">
+        <v>0</v>
+      </c>
+      <c r="G14" s="42"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="42"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="44"/>
-      <c r="B15" s="48" t="s">
+      <c r="A15" s="50"/>
+      <c r="B15" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="49">
+      <c r="C15" s="44">
         <v>45990</v>
       </c>
-      <c r="D15" s="45">
-        <v>0</v>
-      </c>
-      <c r="E15" s="47"/>
-      <c r="F15" s="45">
-        <v>0</v>
-      </c>
-      <c r="G15" s="47"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="47"/>
+      <c r="D15" s="40">
+        <v>0</v>
+      </c>
+      <c r="E15" s="42"/>
+      <c r="F15" s="40">
+        <v>0</v>
+      </c>
+      <c r="G15" s="42"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="42"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="44"/>
-      <c r="B16" s="50" t="s">
+      <c r="A16" s="50"/>
+      <c r="B16" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="51">
+      <c r="C16" s="46">
         <v>45991</v>
       </c>
-      <c r="D16" s="52">
-        <v>0</v>
-      </c>
-      <c r="E16" s="53">
+      <c r="D16" s="47">
+        <v>0</v>
+      </c>
+      <c r="E16" s="48">
         <f>SUM(D10:D16)</f>
         <v>0</v>
       </c>
-      <c r="F16" s="52">
-        <v>0</v>
-      </c>
-      <c r="G16" s="53">
+      <c r="F16" s="47">
+        <v>0</v>
+      </c>
+      <c r="G16" s="48">
         <f>SUM(F10:F16)</f>
         <v>0</v>
       </c>
-      <c r="H16" s="52"/>
-      <c r="I16" s="53">
+      <c r="H16" s="47"/>
+      <c r="I16" s="48">
         <f>SUM(H10:H16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="49" t="s">
         <v>13</v>
       </c>
       <c r="B17" t="s">
@@ -1495,13 +1506,13 @@
         <v>6</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="H17" s="38">
+      <c r="H17">
         <v>2</v>
       </c>
       <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="36"/>
+      <c r="A18" s="49"/>
       <c r="B18" t="s">
         <v>2</v>
       </c>
@@ -1516,13 +1527,13 @@
         <v>5</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="H18" s="38">
+      <c r="H18">
         <v>5</v>
       </c>
       <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="36"/>
+      <c r="A19" s="49"/>
       <c r="B19" t="s">
         <v>3</v>
       </c>
@@ -1537,13 +1548,13 @@
         <v>5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="H19" s="38">
+      <c r="H19">
         <v>4</v>
       </c>
       <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="36"/>
+      <c r="A20" s="49"/>
       <c r="B20" t="s">
         <v>4</v>
       </c>
@@ -1558,13 +1569,13 @@
         <v>6</v>
       </c>
       <c r="G20" s="7"/>
-      <c r="H20" s="38">
+      <c r="H20">
         <v>4</v>
       </c>
       <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="36"/>
+      <c r="A21" s="49"/>
       <c r="B21" t="s">
         <v>5</v>
       </c>
@@ -1582,7 +1593,7 @@
       <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="36"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="10" t="s">
         <v>6</v>
       </c>
@@ -1600,7 +1611,7 @@
       <c r="I22" s="7"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="36"/>
+      <c r="A23" s="49"/>
       <c r="B23" s="12" t="s">
         <v>7</v>
       </c>
@@ -1628,7 +1639,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="49" t="s">
         <v>14</v>
       </c>
       <c r="B24" t="s">
@@ -1637,7 +1648,7 @@
       <c r="C24" s="1">
         <v>45999</v>
       </c>
-      <c r="D24" s="38">
+      <c r="D24">
         <v>6</v>
       </c>
       <c r="E24" s="7"/>
@@ -1645,20 +1656,20 @@
         <v>5</v>
       </c>
       <c r="G24" s="7"/>
-      <c r="H24" s="38">
+      <c r="H24">
         <v>5</v>
       </c>
       <c r="I24" s="7"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="36"/>
+      <c r="A25" s="49"/>
       <c r="B25" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="1">
         <v>46000</v>
       </c>
-      <c r="D25" s="38">
+      <c r="D25">
         <v>5</v>
       </c>
       <c r="E25" s="7"/>
@@ -1666,20 +1677,20 @@
         <v>6</v>
       </c>
       <c r="G25" s="7"/>
-      <c r="H25" s="38">
+      <c r="H25">
         <v>5</v>
       </c>
       <c r="I25" s="7"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="36"/>
+      <c r="A26" s="49"/>
       <c r="B26" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="1">
         <v>46001</v>
       </c>
-      <c r="D26" s="38">
+      <c r="D26">
         <v>8</v>
       </c>
       <c r="E26" s="7"/>
@@ -1687,20 +1698,20 @@
         <v>6</v>
       </c>
       <c r="G26" s="7"/>
-      <c r="H26" s="38">
+      <c r="H26">
         <v>5</v>
       </c>
       <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="36"/>
+      <c r="A27" s="49"/>
       <c r="B27" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="1">
         <v>46002</v>
       </c>
-      <c r="D27" s="38">
+      <c r="D27">
         <v>5</v>
       </c>
       <c r="E27" s="7"/>
@@ -1708,20 +1719,20 @@
         <v>4</v>
       </c>
       <c r="G27" s="7"/>
-      <c r="H27" s="38">
+      <c r="H27">
         <v>5</v>
       </c>
       <c r="I27" s="7"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="36"/>
+      <c r="A28" s="49"/>
       <c r="B28" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="1">
         <v>46003</v>
       </c>
-      <c r="D28" s="38">
+      <c r="D28">
         <v>8</v>
       </c>
       <c r="E28" s="7"/>
@@ -1729,13 +1740,13 @@
         <v>5</v>
       </c>
       <c r="G28" s="7"/>
-      <c r="H28" s="38">
+      <c r="H28">
         <v>5</v>
       </c>
       <c r="I28" s="7"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="36"/>
+      <c r="A29" s="49"/>
       <c r="B29" s="10" t="s">
         <v>6</v>
       </c>
@@ -1750,7 +1761,7 @@
       <c r="I29" s="7"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="36"/>
+      <c r="A30" s="49"/>
       <c r="B30" s="10" t="s">
         <v>7</v>
       </c>
@@ -1771,7 +1782,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="49" t="s">
         <v>15</v>
       </c>
       <c r="B31" t="s">
@@ -1796,7 +1807,7 @@
       <c r="I31" s="7"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="36"/>
+      <c r="A32" s="49"/>
       <c r="B32" t="s">
         <v>2</v>
       </c>
@@ -1819,7 +1830,7 @@
       <c r="I32" s="7"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
+      <c r="A33" s="49"/>
       <c r="B33" t="s">
         <v>3</v>
       </c>
@@ -1834,13 +1845,13 @@
         <v>4</v>
       </c>
       <c r="G33" s="7"/>
-      <c r="H33" s="38">
+      <c r="H33">
         <v>4</v>
       </c>
       <c r="I33" s="7"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="36"/>
+      <c r="A34" s="49"/>
       <c r="B34" t="s">
         <v>4</v>
       </c>
@@ -1852,7 +1863,7 @@
       <c r="I34" s="7"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="36"/>
+      <c r="A35" s="49"/>
       <c r="B35" t="s">
         <v>5</v>
       </c>
@@ -1864,7 +1875,7 @@
       <c r="I35" s="7"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="36"/>
+      <c r="A36" s="49"/>
       <c r="B36" s="10" t="s">
         <v>6</v>
       </c>
@@ -1876,7 +1887,7 @@
       <c r="I36" s="7"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="37"/>
+      <c r="A37" s="51"/>
       <c r="B37" s="12" t="s">
         <v>7</v>
       </c>

</xml_diff>